<commit_message>
frist test case files created.
</commit_message>
<xml_diff>
--- a/Excel/appium_data.xlsx
+++ b/Excel/appium_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/animeshmukherjee/PycharmProjects/pythonProject/Appium_Page_Object_Model/Excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6169E445-3E30-904D-837B-D31C536C850B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE7CF24A-D9AC-EC4A-BE07-072B612B350F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="18980" xr2:uid="{E4A251DD-F0BA-B24E-BB12-1E97DEE930FB}"/>
   </bookViews>
@@ -25,24 +25,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>city</t>
-  </si>
-  <si>
-    <t>country</t>
   </si>
   <si>
     <t>Dubai</t>
   </si>
   <si>
-    <t>UAE</t>
-  </si>
-  <si>
     <t>Delhi</t>
-  </si>
-  <si>
-    <t>India</t>
   </si>
 </sst>
 </file>
@@ -394,36 +385,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8478BAE6-A361-1E40-9CAB-1DC3B60222B5}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C40" sqref="C40"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>2</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
first test case files created.
</commit_message>
<xml_diff>
--- a/Excel/appium_data.xlsx
+++ b/Excel/appium_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/animeshmukherjee/PycharmProjects/pythonProject/Appium_Page_Object_Model/Excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE7CF24A-D9AC-EC4A-BE07-072B612B350F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6213FC0-CBE1-6146-BE4B-A86CD31B9330}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="18980" xr2:uid="{E4A251DD-F0BA-B24E-BB12-1E97DEE930FB}"/>
   </bookViews>
@@ -388,7 +388,7 @@
   <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -400,12 +400,12 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Second test case COMPLETED.
</commit_message>
<xml_diff>
--- a/Excel/appium_data.xlsx
+++ b/Excel/appium_data.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/animeshmukherjee/PycharmProjects/pythonProject/Appium_Page_Object_Model/Excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6213FC0-CBE1-6146-BE4B-A86CD31B9330}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77E85A07-D832-8248-9ECF-5BE7215D9367}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="18980" xr2:uid="{E4A251DD-F0BA-B24E-BB12-1E97DEE930FB}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="18980" activeTab="1" xr2:uid="{E4A251DD-F0BA-B24E-BB12-1E97DEE930FB}"/>
   </bookViews>
   <sheets>
     <sheet name="LoginTest" sheetId="1" r:id="rId1"/>
+    <sheet name="VillaTest" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="6">
   <si>
     <t>city</t>
   </si>
@@ -34,6 +35,15 @@
   </si>
   <si>
     <t>Delhi</t>
+  </si>
+  <si>
+    <t>villa</t>
+  </si>
+  <si>
+    <t>Hotel Saffron</t>
+  </si>
+  <si>
+    <t>Deira Suites</t>
   </si>
 </sst>
 </file>
@@ -387,8 +397,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8478BAE6-A361-1E40-9CAB-1DC3B60222B5}">
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -411,4 +421,43 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E18EA071-6A31-024D-939A-0E99E4FDC5F9}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>